<commit_message>
Upload Readme File For Database
</commit_message>
<xml_diff>
--- a/db/东方M-1漫才统计表.xlsx
+++ b/db/东方M-1漫才统计表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\东JO共荣\东方\M-1\新建文件夹\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4A52CE-606D-4D75-932A-72FD8406AA79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D044E6A-7E1D-4DE9-9616-3A40A7993010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B4F54570-192A-490C-A976-F5082225062F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="129">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3265,8 +3265,8 @@
       <c r="K57" s="1">
         <v>3</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>10</v>
+      <c r="L57" s="1">
+        <v>4</v>
       </c>
       <c r="M57" s="1">
         <v>2</v>
@@ -3306,8 +3306,8 @@
       <c r="K58" s="1">
         <v>2</v>
       </c>
-      <c r="L58" s="1" t="s">
-        <v>10</v>
+      <c r="L58" s="1">
+        <v>3</v>
       </c>
       <c r="M58" s="1">
         <v>3</v>
@@ -3347,8 +3347,8 @@
       <c r="K59" s="1">
         <v>1</v>
       </c>
-      <c r="L59" s="1" t="s">
-        <v>10</v>
+      <c r="L59" s="1">
+        <v>1</v>
       </c>
       <c r="M59" s="1">
         <v>4</v>
@@ -3388,8 +3388,8 @@
       <c r="K60" s="1">
         <v>4</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>10</v>
+      <c r="L60" s="1">
+        <v>2</v>
       </c>
       <c r="M60" s="1">
         <v>5</v>

</xml_diff>